<commit_message>
Initial firmware sync and updated android app
</commit_message>
<xml_diff>
--- a/PCB/BOM.xlsx
+++ b/PCB/BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Documents\SparkSofa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Documents\GitHub\SparkSofa\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -50,9 +50,6 @@
     <t>Relay diode</t>
   </si>
   <si>
-    <t>Resistor (transistor)</t>
-  </si>
-  <si>
     <t>Plugs</t>
   </si>
   <si>
@@ -132,6 +129,9 @@
   </si>
   <si>
     <t>628-8931</t>
+  </si>
+  <si>
+    <t>Resistor 2.2K (transistor)</t>
   </si>
 </sst>
 </file>
@@ -224,7 +224,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -242,23 +241,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -302,6 +285,23 @@
     <dxf>
       <font>
         <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
       </font>
     </dxf>
   </dxfs>
@@ -324,12 +324,12 @@
     <sortCondition ref="C3:C19"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="Item" totalsRowLabel="Total" dataDxfId="7" totalsRowDxfId="3"/>
-    <tableColumn id="2" name="Quantity" totalsRowFunction="sum" dataDxfId="6" totalsRowDxfId="2"/>
+    <tableColumn id="1" name="Item" totalsRowLabel="Total" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="2" name="Quantity" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="4"/>
     <tableColumn id="4" name="Supplier"/>
     <tableColumn id="5" name="Order Code"/>
-    <tableColumn id="6" name="Price" dataDxfId="5" totalsRowDxfId="1" dataCellStyle="Currency"/>
-    <tableColumn id="7" name="Total" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="0" dataCellStyle="Currency">
+    <tableColumn id="6" name="Price" dataDxfId="3" totalsRowDxfId="2" dataCellStyle="Currency"/>
+    <tableColumn id="7" name="Total" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0" dataCellStyle="Currency">
       <calculatedColumnFormula>B4*E4</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -602,14 +602,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="56.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -639,13 +643,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="2">
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E4" s="1">
         <v>8.4000000000000005E-2</v>
@@ -657,16 +661,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="2">
         <v>7</v>
       </c>
       <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
         <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>20</v>
       </c>
       <c r="E5" s="1">
         <v>3.12</v>
@@ -684,10 +688,10 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E6" s="1">
         <v>0</v>
@@ -699,16 +703,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2">
         <v>3</v>
       </c>
       <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
         <v>23</v>
-      </c>
-      <c r="D7" t="s">
-        <v>24</v>
       </c>
       <c r="E7" s="1">
         <v>0.28599999999999998</v>
@@ -720,16 +724,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="2">
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8" s="1">
         <v>0.8</v>
@@ -741,16 +745,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="2">
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E9" s="1">
         <v>0.55000000000000004</v>
@@ -762,16 +766,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="2">
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E10" s="1">
         <v>1.7</v>
@@ -783,16 +787,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="2">
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E11" s="1">
         <v>0.48099999999999998</v>
@@ -804,16 +808,16 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" s="2">
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E12" s="1">
         <v>0</v>
@@ -825,16 +829,16 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="2">
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E13" s="1">
         <v>0</v>
@@ -846,7 +850,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="B14" s="2">
         <v>7</v>
@@ -861,7 +865,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" s="2">
         <v>1</v>
@@ -876,7 +880,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B16" s="2">
         <v>1</v>
@@ -891,7 +895,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B17" s="2">
         <v>1</v>
@@ -906,13 +910,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="2">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E18" s="1">
         <v>0</v>
@@ -924,7 +928,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="2">
         <v>1</v>

</xml_diff>